<commit_message>
parellel exxecution with extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/DataProvider.xlsx
+++ b/src/test/resources/DataProvider.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sagar Sapkal\eclipse-workspace\2022_TestNGFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDAFF02-5849-4743-BDFD-B188682AB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE148277-D76D-4C82-9A46-70CD583EDF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -408,9 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -481,9 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528D18D9-86EF-43BC-AAE1-C9C28415D2FC}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -537,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9DC06E-7598-4B2D-8076-214D10F24F88}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>